<commit_message>
Data from url moved to databases
</commit_message>
<xml_diff>
--- a/dbs/tmp.xlsx
+++ b/dbs/tmp.xlsx
@@ -87,289 +87,321 @@
     </x:row>
     <x:row r="2">
       <x:c r="A2" s="3" t="n">
-        <x:v>1</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="B2" s="4">
-        <x:v>44595</x:v>
+        <x:v>44597</x:v>
       </x:c>
       <x:c r="C2" s="5" t="n">
-        <x:v>76.4849</x:v>
+        <x:v>66.0766</x:v>
       </x:c>
       <x:c r="D2" s="0" t="inlineStr">
         <x:is>
-          <x:t>Доллар США</x:t>
+          <x:t>Японская иена</x:t>
         </x:is>
       </x:c>
     </x:row>
     <x:row r="3">
       <x:c r="A3" s="3" t="n">
-        <x:v>1</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="B3" s="4">
-        <x:v>44594</x:v>
+        <x:v>44596</x:v>
       </x:c>
       <x:c r="C3" s="5" t="n">
-        <x:v>77.1302</x:v>
+        <x:v>66.8412</x:v>
       </x:c>
       <x:c r="D3" s="0" t="inlineStr">
         <x:is>
-          <x:t>Доллар США</x:t>
+          <x:t>Японская иена</x:t>
         </x:is>
       </x:c>
     </x:row>
     <x:row r="4">
       <x:c r="A4" s="3" t="n">
-        <x:v>1</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="B4" s="4">
-        <x:v>44593</x:v>
+        <x:v>44595</x:v>
       </x:c>
       <x:c r="C4" s="5" t="n">
-        <x:v>77.4702</x:v>
+        <x:v>66.7786</x:v>
       </x:c>
       <x:c r="D4" s="0" t="inlineStr">
         <x:is>
-          <x:t>Доллар США</x:t>
+          <x:t>Японская иена</x:t>
         </x:is>
       </x:c>
     </x:row>
     <x:row r="5">
       <x:c r="A5" s="3" t="n">
-        <x:v>1</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="B5" s="4">
-        <x:v>44590</x:v>
+        <x:v>44594</x:v>
       </x:c>
       <x:c r="C5" s="5" t="n">
-        <x:v>77.8174</x:v>
+        <x:v>67.0552</x:v>
       </x:c>
       <x:c r="D5" s="0" t="inlineStr">
         <x:is>
-          <x:t>Доллар США</x:t>
+          <x:t>Японская иена</x:t>
         </x:is>
       </x:c>
     </x:row>
     <x:row r="6">
       <x:c r="A6" s="3" t="n">
-        <x:v>1</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="B6" s="4">
-        <x:v>44589</x:v>
+        <x:v>44593</x:v>
       </x:c>
       <x:c r="C6" s="5" t="n">
-        <x:v>78.9470</x:v>
+        <x:v>67.1523</x:v>
       </x:c>
       <x:c r="D6" s="0" t="inlineStr">
         <x:is>
-          <x:t>Доллар США</x:t>
+          <x:t>Японская иена</x:t>
         </x:is>
       </x:c>
     </x:row>
     <x:row r="7">
       <x:c r="A7" s="3" t="n">
-        <x:v>1</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="B7" s="4">
-        <x:v>44588</x:v>
+        <x:v>44590</x:v>
       </x:c>
       <x:c r="C7" s="5" t="n">
-        <x:v>78.9437</x:v>
+        <x:v>67.3423</x:v>
       </x:c>
       <x:c r="D7" s="0" t="inlineStr">
         <x:is>
-          <x:t>Доллар США</x:t>
+          <x:t>Японская иена</x:t>
         </x:is>
       </x:c>
     </x:row>
     <x:row r="8">
       <x:c r="A8" s="3" t="n">
-        <x:v>1</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="B8" s="4">
-        <x:v>44587</x:v>
+        <x:v>44589</x:v>
       </x:c>
       <x:c r="C8" s="5" t="n">
-        <x:v>78.6422</x:v>
+        <x:v>68.7422</x:v>
       </x:c>
       <x:c r="D8" s="0" t="inlineStr">
         <x:is>
-          <x:t>Доллар США</x:t>
+          <x:t>Японская иена</x:t>
         </x:is>
       </x:c>
     </x:row>
     <x:row r="9">
       <x:c r="A9" s="3" t="n">
-        <x:v>1</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="B9" s="4">
-        <x:v>44586</x:v>
+        <x:v>44588</x:v>
       </x:c>
       <x:c r="C9" s="5" t="n">
-        <x:v>77.3649</x:v>
+        <x:v>69.2033</x:v>
       </x:c>
       <x:c r="D9" s="0" t="inlineStr">
         <x:is>
-          <x:t>Доллар США</x:t>
+          <x:t>Японская иена</x:t>
         </x:is>
       </x:c>
     </x:row>
     <x:row r="10">
       <x:c r="A10" s="3" t="n">
-        <x:v>1</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="B10" s="4">
-        <x:v>44583</x:v>
+        <x:v>44587</x:v>
       </x:c>
       <x:c r="C10" s="5" t="n">
-        <x:v>76.6903</x:v>
+        <x:v>69.0844</x:v>
       </x:c>
       <x:c r="D10" s="0" t="inlineStr">
         <x:is>
-          <x:t>Доллар США</x:t>
+          <x:t>Японская иена</x:t>
         </x:is>
       </x:c>
     </x:row>
     <x:row r="11">
       <x:c r="A11" s="3" t="n">
-        <x:v>1</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="B11" s="4">
-        <x:v>44582</x:v>
+        <x:v>44586</x:v>
       </x:c>
       <x:c r="C11" s="5" t="n">
-        <x:v>76.4408</x:v>
+        <x:v>68.0460</x:v>
       </x:c>
       <x:c r="D11" s="0" t="inlineStr">
         <x:is>
-          <x:t>Доллар США</x:t>
+          <x:t>Японская иена</x:t>
         </x:is>
       </x:c>
     </x:row>
     <x:row r="12">
       <x:c r="A12" s="3" t="n">
-        <x:v>1</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="B12" s="4">
-        <x:v>44581</x:v>
+        <x:v>44583</x:v>
       </x:c>
       <x:c r="C12" s="5" t="n">
-        <x:v>76.8697</x:v>
+        <x:v>67.3165</x:v>
       </x:c>
       <x:c r="D12" s="0" t="inlineStr">
         <x:is>
-          <x:t>Доллар США</x:t>
+          <x:t>Японская иена</x:t>
         </x:is>
       </x:c>
     </x:row>
     <x:row r="13">
       <x:c r="A13" s="3" t="n">
-        <x:v>1</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="B13" s="4">
-        <x:v>44580</x:v>
+        <x:v>44582</x:v>
       </x:c>
       <x:c r="C13" s="5" t="n">
-        <x:v>76.3347</x:v>
+        <x:v>66.8510</x:v>
       </x:c>
       <x:c r="D13" s="0" t="inlineStr">
         <x:is>
-          <x:t>Доллар США</x:t>
+          <x:t>Японская иена</x:t>
         </x:is>
       </x:c>
     </x:row>
     <x:row r="14">
       <x:c r="A14" s="3" t="n">
-        <x:v>1</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="B14" s="4">
-        <x:v>44579</x:v>
+        <x:v>44581</x:v>
       </x:c>
       <x:c r="C14" s="5" t="n">
-        <x:v>76.0404</x:v>
+        <x:v>67.1967</x:v>
       </x:c>
       <x:c r="D14" s="0" t="inlineStr">
         <x:is>
-          <x:t>Доллар США</x:t>
+          <x:t>Японская иена</x:t>
         </x:is>
       </x:c>
     </x:row>
     <x:row r="15">
       <x:c r="A15" s="3" t="n">
-        <x:v>1</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="B15" s="4">
-        <x:v>44576</x:v>
+        <x:v>44580</x:v>
       </x:c>
       <x:c r="C15" s="5" t="n">
-        <x:v>75.7668</x:v>
+        <x:v>66.5429</x:v>
       </x:c>
       <x:c r="D15" s="0" t="inlineStr">
         <x:is>
-          <x:t>Доллар США</x:t>
+          <x:t>Японская иена</x:t>
         </x:is>
       </x:c>
     </x:row>
     <x:row r="16">
       <x:c r="A16" s="3" t="n">
-        <x:v>1</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="B16" s="4">
-        <x:v>44575</x:v>
+        <x:v>44579</x:v>
       </x:c>
       <x:c r="C16" s="5" t="n">
-        <x:v>74.5686</x:v>
+        <x:v>66.5067</x:v>
       </x:c>
       <x:c r="D16" s="0" t="inlineStr">
         <x:is>
-          <x:t>Доллар США</x:t>
+          <x:t>Японская иена</x:t>
         </x:is>
       </x:c>
     </x:row>
     <x:row r="17">
       <x:c r="A17" s="3" t="n">
-        <x:v>1</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="B17" s="4">
-        <x:v>44574</x:v>
+        <x:v>44576</x:v>
       </x:c>
       <x:c r="C17" s="5" t="n">
-        <x:v>74.5277</x:v>
+        <x:v>66.5935</x:v>
       </x:c>
       <x:c r="D17" s="0" t="inlineStr">
         <x:is>
-          <x:t>Доллар США</x:t>
+          <x:t>Японская иена</x:t>
         </x:is>
       </x:c>
     </x:row>
     <x:row r="18">
       <x:c r="A18" s="3" t="n">
-        <x:v>1</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="B18" s="4">
-        <x:v>44573</x:v>
+        <x:v>44575</x:v>
       </x:c>
       <x:c r="C18" s="5" t="n">
-        <x:v>74.8355</x:v>
+        <x:v>65.1624</x:v>
       </x:c>
       <x:c r="D18" s="0" t="inlineStr">
         <x:is>
-          <x:t>Доллар США</x:t>
+          <x:t>Японская иена</x:t>
         </x:is>
       </x:c>
     </x:row>
     <x:row r="19">
       <x:c r="A19" s="3" t="n">
-        <x:v>1</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="B19" s="4">
+        <x:v>44574</x:v>
+      </x:c>
+      <x:c r="C19" s="5" t="n">
+        <x:v>64.5905</x:v>
+      </x:c>
+      <x:c r="D19" s="0" t="inlineStr">
+        <x:is>
+          <x:t>Японская иена</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="20">
+      <x:c r="A20" s="3" t="n">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="B20" s="4">
+        <x:v>44573</x:v>
+      </x:c>
+      <x:c r="C20" s="5" t="n">
+        <x:v>64.9360</x:v>
+      </x:c>
+      <x:c r="D20" s="0" t="inlineStr">
+        <x:is>
+          <x:t>Японская иена</x:t>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="21">
+      <x:c r="A21" s="3" t="n">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="B21" s="4">
         <x:v>44572</x:v>
       </x:c>
-      <x:c r="C19" s="5" t="n">
-        <x:v>75.1315</x:v>
-      </x:c>
-      <x:c r="D19" s="0" t="inlineStr">
-        <x:is>
-          <x:t>Доллар США</x:t>
+      <x:c r="C21" s="5" t="n">
+        <x:v>64.9168</x:v>
+      </x:c>
+      <x:c r="D21" s="0" t="inlineStr">
+        <x:is>
+          <x:t>Японская иена</x:t>
         </x:is>
       </x:c>
     </x:row>

</xml_diff>